<commit_message>
data provider done in dummytest1
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelData/Data.xlsx
+++ b/src/test/resources/ExcelData/Data.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\falca\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zvijayfa\eclipse-workspace\edureka-automation-testing\src\test\resources\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1294E2C8-F847-4742-96F7-894FA643AA6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778CB3C7-85BF-4C36-BFDB-985D511DFD0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="4" xr2:uid="{7EAF6881-DA24-4AF8-A0BA-FB8E17B54B3B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{7EAF6881-DA24-4AF8-A0BA-FB8E17B54B3B}"/>
   </bookViews>
   <sheets>
     <sheet name="WebinarTestData" sheetId="1" r:id="rId1"/>
     <sheet name="JobApplicationData" sheetId="2" r:id="rId2"/>
-    <sheet name="SearchTestData" sheetId="3" r:id="rId3"/>
-    <sheet name="NavigationTestData" sheetId="4" r:id="rId4"/>
-    <sheet name="FormValidationData" sheetId="5" r:id="rId5"/>
+    <sheet name="SearchTestData2" sheetId="3" r:id="rId3"/>
+    <sheet name="SearchTestData" sheetId="6" r:id="rId4"/>
+    <sheet name="NavigationTestData" sheetId="4" r:id="rId5"/>
+    <sheet name="FormValidationData" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="71">
   <si>
     <t>WebinarName</t>
   </si>
@@ -90,30 +91,9 @@
     <t>DevOps</t>
   </si>
   <si>
-    <t>Job Title</t>
-  </si>
-  <si>
-    <t>Applicant Name</t>
-  </si>
-  <si>
-    <t>Applicant Email</t>
-  </si>
-  <si>
-    <t>Applicant Phone</t>
-  </si>
-  <si>
-    <t>Expected Result</t>
-  </si>
-  <si>
-    <t>Associate Research Analyst</t>
-  </si>
-  <si>
     <t>Zane Falcao</t>
   </si>
   <si>
-    <t>zanefalcao@test.com</t>
-  </si>
-  <si>
     <t>John Doe</t>
   </si>
   <si>
@@ -156,9 +136,6 @@
     <t>TestDescription</t>
   </si>
   <si>
-    <t>Java</t>
-  </si>
-  <si>
     <t>Valid search with results</t>
   </si>
   <si>
@@ -210,18 +187,6 @@
     <t>/careers</t>
   </si>
   <si>
-    <t>All Courses</t>
-  </si>
-  <si>
-    <t>/all-courses</t>
-  </si>
-  <si>
-    <t>Blog</t>
-  </si>
-  <si>
-    <t>/blog</t>
-  </si>
-  <si>
     <t>FieldName</t>
   </si>
   <si>
@@ -262,6 +227,33 @@
   </si>
   <si>
     <t>Name too short</t>
+  </si>
+  <si>
+    <t>zanefalcao21@gmail.com</t>
+  </si>
+  <si>
+    <t>agentic ai</t>
+  </si>
+  <si>
+    <t>cyber security</t>
+  </si>
+  <si>
+    <t>hwchwvhenov</t>
+  </si>
+  <si>
+    <t>aws</t>
+  </si>
+  <si>
+    <t>azure</t>
+  </si>
+  <si>
+    <t>ApplicantEmail</t>
+  </si>
+  <si>
+    <t>ApplicantPhone</t>
+  </si>
+  <si>
+    <t>ApplicantName</t>
   </si>
 </sst>
 </file>
@@ -670,17 +662,17 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="1" max="2" width="17.54296875" customWidth="1"/>
+    <col min="3" max="3" width="13.7265625" customWidth="1"/>
+    <col min="4" max="4" width="15.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -694,7 +686,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -708,7 +700,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -722,7 +714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -736,7 +728,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -750,7 +742,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -764,7 +756,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -785,104 +777,72 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{742909C5-CA6D-49AE-966B-68E13DE41584}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="30.42578125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" customWidth="1"/>
+    <col min="2" max="2" width="22.26953125" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>4</v>
+        <v>22</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -896,34 +856,34 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" customWidth="1"/>
+    <col min="4" max="4" width="24.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="B2" s="4">
         <v>10</v>
@@ -932,12 +892,12 @@
         <v>7</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B3" s="4">
         <v>15</v>
@@ -946,10 +906,10 @@
         <v>7</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -960,12 +920,12 @@
         <v>7</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B5" s="4">
         <v>0</v>
@@ -974,12 +934,12 @@
         <v>10</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B6" s="4">
         <v>12</v>
@@ -988,10 +948,10 @@
         <v>7</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1002,7 +962,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1011,83 +971,46 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E67122A-25E8-4B7D-9D5F-D1C40D93341B}">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B48E8B2F-9CDF-4B22-99C6-014ABE6124CD}">
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1096,64 +1019,121 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E67122A-25E8-4B7D-9D5F-D1C40D93341B}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C76D2BE6-0DCB-40AA-8DFA-CCCEF0E852FA}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B4" s="1">
         <v>9876543210</v>
@@ -1162,12 +1142,12 @@
         <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B5" s="4">
         <v>12345</v>
@@ -1176,35 +1156,35 @@
         <v>10</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>